<commit_message>
Flash erase status added
</commit_message>
<xml_diff>
--- a/Wifi bootloader prelim CPD.xlsx
+++ b/Wifi bootloader prelim CPD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Neil\Dropbox (Mernok Elektronik)\Software\WIFI app\WIFI Config App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94110A5-3382-4A9B-A9CC-44F838814F94}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86420DE3-07B3-40AC-AD91-66394FAF3CA0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24810" windowHeight="7320" xr2:uid="{40E3CE3B-EF58-486E-AF0D-E47A9341A25D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="36">
   <si>
     <t>SOF1</t>
   </si>
@@ -126,16 +126,19 @@
     <t>h</t>
   </si>
   <si>
-    <t>count1</t>
-  </si>
-  <si>
-    <t>count2</t>
-  </si>
-  <si>
-    <t>count3</t>
-  </si>
-  <si>
-    <t>count4</t>
+    <t>r</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>bootinfo5</t>
+  </si>
+  <si>
+    <t>bootinfo6</t>
   </si>
 </sst>
 </file>
@@ -227,9 +230,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -237,6 +237,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -553,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A892C028-128A-40A3-B6C1-B141BD38CF44}">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,10 +573,11 @@
     <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>17</v>
       </c>
@@ -589,45 +593,47 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
     </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6">
         <v>0</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>1</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>2</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>3</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <v>4</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="6">
         <v>5</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="6">
         <v>6</v>
       </c>
       <c r="J2" s="1">
@@ -642,158 +648,170 @@
       <c r="M2" s="1">
         <v>10</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="1">
+        <v>11</v>
+      </c>
+      <c r="O2" s="1">
+        <v>12</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="1">
+      <c r="Q2" s="1">
         <v>520</v>
       </c>
-      <c r="P2" s="1">
+      <c r="R2" s="1">
         <v>521</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="S2" s="1">
         <v>522</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>522</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="K3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="L3" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="2">
+      <c r="M3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="2">
         <v>0</v>
       </c>
-      <c r="L3" s="2">
-        <v>0</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0</v>
-      </c>
-      <c r="O3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <f>COUNTA(C4:M4)</f>
         <v>7</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <f>COUNTA(C5:M5)</f>
         <v>7</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>522</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="5" t="s">
         <v>15</v>
       </c>
       <c r="J6" s="2" t="s">
@@ -809,45 +827,51 @@
         <v>23</v>
       </c>
       <c r="N6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="Q6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="R6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="S6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <f>COUNTA(C7:M7)</f>
         <v>11</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="5" t="s">
         <v>14</v>
       </c>
       <c r="J7" s="2" t="s">
@@ -862,40 +886,42 @@
       <c r="M7" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <f>COUNTA(C8:K8)</f>
         <v>7</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="5" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F1:Q1"/>
+    <mergeCell ref="F1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>